<commit_message>
Added test case names and path for DmsDocumentLibrary DMS_SmartFolder DMS_CreateView DMS_TransmittalFolderView
</commit_message>
<xml_diff>
--- a/Fulcrum_PreProd_Trunk/src/com/proj/config/Config.xlsx
+++ b/Fulcrum_PreProd_Trunk/src/com/proj/config/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14865" windowHeight="2820" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14865" windowHeight="2820"/>
   </bookViews>
   <sheets>
     <sheet name="DataFetchFlag" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="13">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>\\src\\com\\proj\\suiteDOCS\\testdata\\DmsDocumentLibrary.xlsx</t>
+  </si>
+  <si>
+    <t>DMS_SmartFolder</t>
+  </si>
+  <si>
+    <t>DMS_CreateView</t>
+  </si>
+  <si>
+    <t>DMS_TransmittalFolderView</t>
   </si>
 </sst>
 </file>
@@ -510,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -545,13 +554,28 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="B4" s="3"/>
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="B5" s="3"/>
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="B6" s="3"/>
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:2">
       <c r="B7" s="3"/>
@@ -614,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -659,13 +683,37 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="B4" s="2"/>
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="B5" s="2"/>
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="B6" s="2"/>
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="B7" s="2"/>
@@ -716,10 +764,13 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added test case and path for DMS_SmartFolder DMS_CreateView DMS_TransmittalFolderView
</commit_message>
<xml_diff>
--- a/Fulcrum_PreProd_Trunk/src/com/proj/config/Config.xlsx
+++ b/Fulcrum_PreProd_Trunk/src/com/proj/config/Config.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="18">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -88,12 +88,36 @@
   </si>
   <si>
     <t>\\src\\com\\proj\\suiteDOCS\\testdata\\DmsDocumentLibrary.xlsx</t>
+  </si>
+  <si>
+    <t>FUL_Transmittals_ActionRequired_New_ChangeNote</t>
+  </si>
+  <si>
+    <t>FUL_Transmittals_ActionOverDue_New_ChangeNote</t>
+  </si>
+  <si>
+    <t>\\src\\com\\proj\\suiteTRANSMITTALS\\testdata\\TransmittalsTestData-ChangeNote.xlsx</t>
+  </si>
+  <si>
+    <t>Transmittals_New_ActionRequired</t>
+  </si>
+  <si>
+    <t>Transmittals_New_ActionOverDue</t>
+  </si>
+  <si>
+    <t>DMS_SmartFolder</t>
+  </si>
+  <si>
+    <t>DMS_CreateView</t>
+  </si>
+  <si>
+    <t>DMS_TransmittalFolderView</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -508,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A4" sqref="A4:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -545,19 +569,44 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="B4" s="3"/>
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="B5" s="3"/>
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="B6" s="3"/>
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="B7" s="3"/>
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="B8" s="3"/>
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:2">
       <c r="B9" s="3"/>
@@ -598,9 +647,18 @@
     <row r="21" spans="2:2">
       <c r="B21" s="3"/>
     </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="3"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B24">
       <formula1>"XL,DB"</formula1>
     </dataValidation>
   </dataValidations>
@@ -612,15 +670,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="46.7109375" customWidth="1"/>
+    <col min="1" max="1" width="49.140625" customWidth="1"/>
     <col min="2" max="2" width="109.5703125" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
   </cols>
@@ -659,19 +717,59 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="B4" s="2"/>
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="B5" s="2"/>
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="B6" s="2"/>
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="B7" s="2"/>
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="B8" s="2"/>
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:3">
       <c r="B9" s="2"/>
@@ -711,15 +809,29 @@
     </row>
     <row r="21" spans="2:2">
       <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B7" r:id="rId3"/>
+    <hyperlink ref="B8" r:id="rId4"/>
+    <hyperlink ref="B4" r:id="rId5"/>
+    <hyperlink ref="B5" r:id="rId6"/>
+    <hyperlink ref="B6" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>